<commit_message>
Cost Saving (CS) Algorithm fix, groups graph
</commit_message>
<xml_diff>
--- a/data/Datos.xlsx
+++ b/data/Datos.xlsx
@@ -1,32 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninfa\Documents\TFG\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernando/PycharmProjects/MOPG_Proyecto2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CD352C-5B08-C141-A3B8-A7A1688A4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residuos2014" sheetId="3" r:id="rId1"/>
-    <sheet name="Distancias" sheetId="2" r:id="rId2"/>
-    <sheet name="Produccion de Reiduos" sheetId="1" r:id="rId3"/>
+    <sheet name="Coordenadas" sheetId="4" r:id="rId2"/>
+    <sheet name="Distancias" sheetId="2" r:id="rId3"/>
+    <sheet name="Produccion de Reiduos" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Coordenadas!$A$1:$A$91</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="101">
   <si>
     <t>MUNICIPIO</t>
   </si>
@@ -324,11 +339,17 @@
   <si>
     <t>?</t>
   </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -864,20 +885,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -885,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -893,7 +914,7 @@
         <v>2168.29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -901,7 +922,7 @@
         <v>1187.82</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -909,7 +930,7 @@
         <v>370.44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -917,7 +938,7 @@
         <v>153.85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -925,7 +946,7 @@
         <v>3301.08</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -933,7 +954,7 @@
         <v>279.86</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -941,7 +962,7 @@
         <v>13576.39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -949,7 +970,7 @@
         <v>8648.27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -957,7 +978,7 @@
         <v>614.71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -965,7 +986,7 @@
         <v>864.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -973,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -981,7 +1002,7 @@
         <v>4758.3500000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -989,7 +1010,7 @@
         <v>794.28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -997,7 +1018,7 @@
         <v>147.46</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +1026,7 @@
         <v>18157.349999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1013,7 +1034,7 @@
         <v>154.80000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -1021,7 +1042,7 @@
         <v>3464.9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
@@ -1029,7 +1050,7 @@
         <v>1093.79</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1037,7 +1058,7 @@
         <v>444.06</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -1045,7 +1066,7 @@
         <v>2155.2800000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -1053,7 +1074,7 @@
         <v>45.89</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -1061,7 +1082,7 @@
         <v>83.38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1090,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>999.64</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1085,7 +1106,7 @@
         <v>989.96</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1093,7 +1114,7 @@
         <v>833.04</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
@@ -1101,7 +1122,7 @@
         <v>287.72000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
@@ -1109,7 +1130,7 @@
         <v>315.86</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1138,7 @@
         <v>701.02</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>36</v>
       </c>
@@ -1125,7 +1146,7 @@
         <v>3667.25</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>37</v>
       </c>
@@ -1133,7 +1154,7 @@
         <v>808.51</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>38</v>
       </c>
@@ -1141,7 +1162,7 @@
         <v>311.19</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
@@ -1149,7 +1170,7 @@
         <v>765.82</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1157,7 +1178,7 @@
         <v>344.87</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
@@ -1165,7 +1186,7 @@
         <v>136.03</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>8645.7800000000007</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
@@ -1181,7 +1202,7 @@
         <v>3065.18</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
@@ -1189,7 +1210,7 @@
         <v>1072.3900000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
@@ -1197,7 +1218,7 @@
         <v>8037.34</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
@@ -1205,7 +1226,7 @@
         <v>915.67</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>485.72</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -1221,7 +1242,7 @@
         <v>791.31</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -1229,7 +1250,7 @@
         <v>1118.47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -1237,7 +1258,7 @@
         <v>594.66999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
@@ -1245,7 +1266,7 @@
         <v>1457.05</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -1253,7 +1274,7 @@
         <v>720.18</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>53</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>212.18</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>54</v>
       </c>
@@ -1269,7 +1290,7 @@
         <v>133.85</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
@@ -1277,7 +1298,7 @@
         <v>1718.35</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
@@ -1285,7 +1306,7 @@
         <v>1086.33</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
@@ -1293,7 +1314,7 @@
         <v>871.1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>58</v>
       </c>
@@ -1301,7 +1322,7 @@
         <v>161.26</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>59</v>
       </c>
@@ -1309,7 +1330,7 @@
         <v>910.54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>60</v>
       </c>
@@ -1317,7 +1338,7 @@
         <v>1439.47</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>61</v>
       </c>
@@ -1325,7 +1346,7 @@
         <v>447.81</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>62</v>
       </c>
@@ -1333,7 +1354,7 @@
         <v>302.7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>63</v>
       </c>
@@ -1341,7 +1362,7 @@
         <v>148.97999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>64</v>
       </c>
@@ -1349,7 +1370,7 @@
         <v>230.09</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>65</v>
       </c>
@@ -1357,7 +1378,7 @@
         <v>130.04</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>66</v>
       </c>
@@ -1365,7 +1386,7 @@
         <v>160.5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
@@ -1373,7 +1394,7 @@
         <v>411.84</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>68</v>
       </c>
@@ -1381,7 +1402,7 @@
         <v>2175.9899999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -1389,7 +1410,7 @@
         <v>950.01</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>70</v>
       </c>
@@ -1397,7 +1418,7 @@
         <v>549.55999999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
@@ -1405,7 +1426,7 @@
         <v>13440.41</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>72</v>
       </c>
@@ -1413,7 +1434,7 @@
         <v>131.13</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>73</v>
       </c>
@@ -1421,7 +1442,7 @@
         <v>1058.1500000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>74</v>
       </c>
@@ -1429,7 +1450,7 @@
         <v>3316.08</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>75</v>
       </c>
@@ -1437,7 +1458,7 @@
         <v>170.85</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>76</v>
       </c>
@@ -1445,7 +1466,7 @@
         <v>18258.63</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>77</v>
       </c>
@@ -1453,7 +1474,7 @@
         <v>921.03</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>78</v>
       </c>
@@ -1461,7 +1482,7 @@
         <v>19949.990000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>79</v>
       </c>
@@ -1469,7 +1490,7 @@
         <v>72.790000000000006</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>80</v>
       </c>
@@ -1477,7 +1498,7 @@
         <v>498.41</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>81</v>
       </c>
@@ -1485,7 +1506,7 @@
         <v>227.27</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>82</v>
       </c>
@@ -1493,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>83</v>
       </c>
@@ -1501,7 +1522,7 @@
         <v>1474.17</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>84</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>1709.16</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>85</v>
       </c>
@@ -1517,7 +1538,7 @@
         <v>899.22</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>86</v>
       </c>
@@ -1525,7 +1546,7 @@
         <v>8869.92</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>87</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>236.25</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>88</v>
       </c>
@@ -1541,7 +1562,7 @@
         <v>997.34</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>89</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>37177.699999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>90</v>
       </c>
@@ -1557,7 +1578,7 @@
         <v>1561.94</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>91</v>
       </c>
@@ -1565,7 +1586,7 @@
         <v>2020.59</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>92</v>
       </c>
@@ -1573,7 +1594,7 @@
         <v>1428.15</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>93</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>638.04999999999995</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>94</v>
       </c>
@@ -1589,7 +1610,7 @@
         <v>2166.91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>95</v>
       </c>
@@ -1597,7 +1618,7 @@
         <v>905.48</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>96</v>
       </c>
@@ -1611,20 +1632,1040 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C168C-B463-FB40-91D4-911233F2EC8B}">
+  <dimension ref="A1:C91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="60.5" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12">
+        <v>37.232003979207903</v>
+      </c>
+      <c r="C2" s="12">
+        <v>-4.6651912840999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>36.904384480831197</v>
+      </c>
+      <c r="C3" s="12">
+        <v>-4.1301718569999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="12">
+        <v>36.988885402548803</v>
+      </c>
+      <c r="C4" s="12">
+        <v>-4.2542294261000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>36.966017318630897</v>
+      </c>
+      <c r="C5" s="12">
+        <v>-4.2635318005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12">
+        <v>36.760731431693202</v>
+      </c>
+      <c r="C6" s="12">
+        <v>-4.0450602259000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>36.575095809672</v>
+      </c>
+      <c r="C7" s="12">
+        <v>-5.2831731604899996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12">
+        <v>36.671883420274597</v>
+      </c>
+      <c r="C8" s="12">
+        <v>-4.5679697737999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12">
+        <v>36.6423851897924</v>
+      </c>
+      <c r="C9" s="12">
+        <v>-4.6907868796000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12">
+        <v>36.831934227411203</v>
+      </c>
+      <c r="C10" s="12">
+        <v>-4.2185084382999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="12">
+        <v>37.023795994833399</v>
+      </c>
+      <c r="C11" s="12">
+        <v>-5.0144108073</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="12">
+        <v>36.836293636830298</v>
+      </c>
+      <c r="C12" s="12">
+        <v>-4.5332563706000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="12">
+        <v>36.836675799885697</v>
+      </c>
+      <c r="C13" s="12">
+        <v>-4.7037755712999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="12">
+        <v>36.738319533178398</v>
+      </c>
+      <c r="C14" s="12">
+        <v>-4.8641290184999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="12">
+        <v>36.646413224726601</v>
+      </c>
+      <c r="C15" s="12">
+        <v>-5.2232595433000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="12">
+        <v>37.054885251042599</v>
+      </c>
+      <c r="C16" s="12">
+        <v>-4.5928281775000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="12">
+        <v>36.827009284864097</v>
+      </c>
+      <c r="C17" s="12">
+        <v>-3.9951508939</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="12">
+        <v>37.099453190791998</v>
+      </c>
+      <c r="C18" s="12">
+        <v>-4.38851560153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="12">
+        <v>36.889874327310899</v>
+      </c>
+      <c r="C19" s="12">
+        <v>-4.8368476731000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="12">
+        <v>36.819348094112399</v>
+      </c>
+      <c r="C20" s="12">
+        <v>-4.0708139706999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="12">
+        <v>36.7973541352046</v>
+      </c>
+      <c r="C21" s="12">
+        <v>-5.1369926552000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="12">
+        <v>36.646568079635699</v>
+      </c>
+      <c r="C22" s="12">
+        <v>-5.2420650448000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="12">
+        <v>36.614924604447801</v>
+      </c>
+      <c r="C23" s="12">
+        <v>-5.2674450215000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="12">
+        <v>36.584467851983398</v>
+      </c>
+      <c r="C24" s="12">
+        <v>-5.3022639993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="12">
+        <v>36.845100752018098</v>
+      </c>
+      <c r="C25" s="12">
+        <v>-4.1957014390999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="12">
+        <v>36.790217000208003</v>
+      </c>
+      <c r="C26" s="12">
+        <v>-4.1642423505700004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="12">
+        <v>36.708666531790598</v>
+      </c>
+      <c r="C27" s="12">
+        <v>-5.2565809267999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="12">
+        <v>36.549085453703398</v>
+      </c>
+      <c r="C28" s="12">
+        <v>-5.3047204372000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="12">
+        <v>36.824997611620603</v>
+      </c>
+      <c r="C29" s="12">
+        <v>-4.2566211361999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="12">
+        <v>36.803935682271401</v>
+      </c>
+      <c r="C30" s="12">
+        <v>-4.9369838534000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="12">
+        <v>37.0029527901888</v>
+      </c>
+      <c r="C31" s="12">
+        <v>-4.8540957096000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12">
+        <v>36.864110376385099</v>
+      </c>
+      <c r="C32" s="12">
+        <v>-4.1008872007999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="12">
+        <v>36.8503886398044</v>
+      </c>
+      <c r="C33" s="12">
+        <v>-3.9793681255000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="12">
+        <v>36.957008930283301</v>
+      </c>
+      <c r="C34" s="12">
+        <v>-5.0433218416000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="12">
+        <v>36.846800347216401</v>
+      </c>
+      <c r="C35" s="12">
+        <v>-4.8217895044999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="12">
+        <v>36.652714282908498</v>
+      </c>
+      <c r="C36" s="12">
+        <v>-5.1511289397000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="12">
+        <v>36.743996229902599</v>
+      </c>
+      <c r="C37" s="12">
+        <v>-4.6679571363000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="12">
+        <v>36.866055199272999</v>
+      </c>
+      <c r="C38" s="12">
+        <v>-4.4268058961800003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="12">
+        <v>36.8017823726424</v>
+      </c>
+      <c r="C39" s="12">
+        <v>-4.8290976841999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="12">
+        <v>36.674499080169497</v>
+      </c>
+      <c r="C40" s="12">
+        <v>-4.7661059513000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="12">
+        <v>36.913604099018301</v>
+      </c>
+      <c r="C41" s="12">
+        <v>-4.3211654614999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="12">
+        <v>36.855554838878703</v>
+      </c>
+      <c r="C42" s="12">
+        <v>-4.2619849681000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="12">
+        <v>36.8333080748342</v>
+      </c>
+      <c r="C43" s="12">
+        <v>-3.9268918953999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="12">
+        <v>36.569483218773101</v>
+      </c>
+      <c r="C44" s="12">
+        <v>-5.4315437812000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="12">
+        <v>37.2300103047166</v>
+      </c>
+      <c r="C45" s="12">
+        <v>-4.4793112420999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="12">
+        <v>37.260723003898903</v>
+      </c>
+      <c r="C46" s="12">
+        <v>-4.4269460173999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="12">
+        <v>36.877296980638398</v>
+      </c>
+      <c r="C47" s="12">
+        <v>-5.0386300213000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="12">
+        <v>36.8654531947358</v>
+      </c>
+      <c r="C48" s="12">
+        <v>-4.2242237673999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="12">
+        <v>36.612446849746597</v>
+      </c>
+      <c r="C49" s="12">
+        <v>-5.1965715469999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="12">
+        <v>36.810269148087897</v>
+      </c>
+      <c r="C50" s="12">
+        <v>-3.8868405198999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="12">
+        <v>37.125904222545898</v>
+      </c>
+      <c r="C51" s="12">
+        <v>-4.7510660087999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="12">
+        <v>36.513129388312699</v>
+      </c>
+      <c r="C52" s="12">
+        <v>-5.3436405285999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="12">
+        <v>36.526313318384403</v>
+      </c>
+      <c r="C53" s="12">
+        <v>-5.2322431797000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="12">
+        <v>36.674054823920201</v>
+      </c>
+      <c r="C54" s="12">
+        <v>-4.8373058526000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="12">
+        <v>37.133257966701599</v>
+      </c>
+      <c r="C55" s="12">
+        <v>-4.6871220062000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="12">
+        <v>36.624797493797999</v>
+      </c>
+      <c r="C56" s="12">
+        <v>-5.09594994384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="12">
+        <v>36.784812600921597</v>
+      </c>
+      <c r="C57" s="12">
+        <v>-4.1879015233999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="12">
+        <v>36.6520122871962</v>
+      </c>
+      <c r="C58" s="12">
+        <v>-5.2806885363999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="12">
+        <v>36.568491049803498</v>
+      </c>
+      <c r="C59" s="12">
+        <v>-5.2186695579000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="12">
+        <v>36.594583839309401</v>
+      </c>
+      <c r="C60" s="12">
+        <v>-5.1560547003000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="12">
+        <v>36.7687108440945</v>
+      </c>
+      <c r="C61" s="12">
+        <v>-4.2215769506000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="12">
+        <v>36.767282832588599</v>
+      </c>
+      <c r="C62" s="12">
+        <v>-4.2608153335000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="12">
+        <v>37.1378450537172</v>
+      </c>
+      <c r="C63" s="12">
+        <v>-4.6412797699999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="12">
+        <v>36.625018146781699</v>
+      </c>
+      <c r="C64" s="12">
+        <v>-4.8475735297</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="12">
+        <v>36.728411172977601</v>
+      </c>
+      <c r="C65" s="12">
+        <v>-5.2851863065</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="12">
+        <v>36.764597700136399</v>
+      </c>
+      <c r="C66" s="12">
+        <v>-3.8399798238999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="12">
+        <v>36.665685191027201</v>
+      </c>
+      <c r="C67" s="12">
+        <v>-5.0820901949000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="12">
+        <v>36.934452426652797</v>
+      </c>
+      <c r="C68" s="12">
+        <v>-4.1868842455999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="12">
+        <v>36.769207247815103</v>
+      </c>
+      <c r="C69" s="12">
+        <v>-4.7013889478999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="12">
+        <v>36.589366858275298</v>
+      </c>
+      <c r="C70" s="12">
+        <v>-5.1375092865000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="12">
+        <v>36.7245684036249</v>
+      </c>
+      <c r="C71" s="12">
+        <v>-4.2710127862</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="12">
+        <v>36.921299999066299</v>
+      </c>
+      <c r="C72" s="12">
+        <v>-4.2859650847999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="12">
+        <v>36.80214801548</v>
+      </c>
+      <c r="C73" s="12">
+        <v>-5.1393441707690002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="12">
+        <v>36.857247396181499</v>
+      </c>
+      <c r="C74" s="12">
+        <v>-4.0155246251000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="12">
+        <v>36.797869780591498</v>
+      </c>
+      <c r="C75" s="12">
+        <v>-4.0054789806000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="12">
+        <v>36.849961221944199</v>
+      </c>
+      <c r="C76" s="12">
+        <v>-4.0554133122999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="12">
+        <v>36.888300000000001</v>
+      </c>
+      <c r="C77" s="12">
+        <v>-4.9744400000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="12">
+        <v>37.161691934331699</v>
+      </c>
+      <c r="C78" s="12">
+        <v>-4.8654806491000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="12">
+        <v>36.972483941198597</v>
+      </c>
+      <c r="C79" s="12">
+        <v>-4.9059021505000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="12">
+        <v>36.675409557681199</v>
+      </c>
+      <c r="C80" s="12">
+        <v>-4.9374076740000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="12">
+        <v>36.757966532036498</v>
+      </c>
+      <c r="C81" s="12">
+        <v>-3.9585537837000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="12">
+        <v>36.760164625647398</v>
+      </c>
+      <c r="C82" s="12">
+        <v>-4.2928930199000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="12">
+        <v>36.9387373481701</v>
+      </c>
+      <c r="C83" s="12">
+        <v>-4.6704258609</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="12">
+        <v>36.760710091655902</v>
+      </c>
+      <c r="C84" s="12">
+        <v>-4.1232077759000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" s="12">
+        <v>37.181072797661599</v>
+      </c>
+      <c r="C85" s="12">
+        <v>-4.4095310029999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="12">
+        <v>36.931100000000001</v>
+      </c>
+      <c r="C86" s="12">
+        <v>-4.5316700000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" s="12">
+        <v>37.009916632371798</v>
+      </c>
+      <c r="C87" s="12">
+        <v>-4.3779554575999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="12">
+        <v>37.185607687703403</v>
+      </c>
+      <c r="C88" s="12">
+        <v>-4.3424655676999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89" s="12">
+        <v>37.047855563301503</v>
+      </c>
+      <c r="C89" s="12">
+        <v>-4.3221103806999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" s="12">
+        <v>36.861582033583502</v>
+      </c>
+      <c r="C90" s="12">
+        <v>-4.1453074069999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="12">
+        <v>36.735426788524201</v>
+      </c>
+      <c r="C91" s="12">
+        <v>-4.9271544535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FL103"/>
   <sheetViews>
     <sheetView topLeftCell="BW83" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="CJ89" sqref="CJ89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:168" s="8" customFormat="1" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:168" s="8" customFormat="1" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1974,7 +3015,7 @@
       <c r="FK1" s="20"/>
       <c r="FL1" s="19"/>
     </row>
-    <row r="2" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -2325,7 +3366,7 @@
       <c r="FJ2" s="21"/>
       <c r="FK2" s="21"/>
     </row>
-    <row r="3" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
@@ -2676,7 +3717,7 @@
       <c r="FJ3" s="21"/>
       <c r="FK3" s="21"/>
     </row>
-    <row r="4" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>9</v>
       </c>
@@ -3027,7 +4068,7 @@
       <c r="FJ4" s="21"/>
       <c r="FK4" s="21"/>
     </row>
-    <row r="5" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -3378,7 +4419,7 @@
       <c r="FJ5" s="21"/>
       <c r="FK5" s="21"/>
     </row>
-    <row r="6" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
@@ -3729,7 +4770,7 @@
       <c r="FJ6" s="21"/>
       <c r="FK6" s="21"/>
     </row>
-    <row r="7" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -4080,7 +5121,7 @@
       <c r="FJ7" s="21"/>
       <c r="FK7" s="21"/>
     </row>
-    <row r="8" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
@@ -4431,7 +5472,7 @@
       <c r="FJ8" s="21"/>
       <c r="FK8" s="21"/>
     </row>
-    <row r="9" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>14</v>
       </c>
@@ -4782,7 +5823,7 @@
       <c r="FJ9" s="21"/>
       <c r="FK9" s="21"/>
     </row>
-    <row r="10" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>15</v>
       </c>
@@ -5133,7 +6174,7 @@
       <c r="FJ10" s="21"/>
       <c r="FK10" s="21"/>
     </row>
-    <row r="11" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
@@ -5484,7 +6525,7 @@
       <c r="FJ11" s="21"/>
       <c r="FK11" s="21"/>
     </row>
-    <row r="12" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>17</v>
       </c>
@@ -5835,7 +6876,7 @@
       <c r="FJ12" s="21"/>
       <c r="FK12" s="21"/>
     </row>
-    <row r="13" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>18</v>
       </c>
@@ -6186,7 +7227,7 @@
       <c r="FJ13" s="21"/>
       <c r="FK13" s="21"/>
     </row>
-    <row r="14" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
@@ -6537,7 +7578,7 @@
       <c r="FJ14" s="21"/>
       <c r="FK14" s="21"/>
     </row>
-    <row r="15" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>20</v>
       </c>
@@ -6888,7 +7929,7 @@
       <c r="FJ15" s="21"/>
       <c r="FK15" s="21"/>
     </row>
-    <row r="16" spans="1:168" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:168" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
@@ -7239,7 +8280,7 @@
       <c r="FJ16" s="21"/>
       <c r="FK16" s="21"/>
     </row>
-    <row r="17" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>22</v>
       </c>
@@ -7590,7 +8631,7 @@
       <c r="FJ17" s="21"/>
       <c r="FK17" s="21"/>
     </row>
-    <row r="18" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>23</v>
       </c>
@@ -7941,7 +8982,7 @@
       <c r="FJ18" s="21"/>
       <c r="FK18" s="21"/>
     </row>
-    <row r="19" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>24</v>
       </c>
@@ -8292,7 +9333,7 @@
       <c r="FJ19" s="21"/>
       <c r="FK19" s="21"/>
     </row>
-    <row r="20" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>25</v>
       </c>
@@ -8643,7 +9684,7 @@
       <c r="FJ20" s="21"/>
       <c r="FK20" s="21"/>
     </row>
-    <row r="21" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>26</v>
       </c>
@@ -8994,7 +10035,7 @@
       <c r="FJ21" s="21"/>
       <c r="FK21" s="21"/>
     </row>
-    <row r="22" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>27</v>
       </c>
@@ -9345,7 +10386,7 @@
       <c r="FJ22" s="21"/>
       <c r="FK22" s="21"/>
     </row>
-    <row r="23" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>28</v>
       </c>
@@ -9696,7 +10737,7 @@
       <c r="FJ23" s="21"/>
       <c r="FK23" s="21"/>
     </row>
-    <row r="24" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>29</v>
       </c>
@@ -10047,7 +11088,7 @@
       <c r="FJ24" s="21"/>
       <c r="FK24" s="21"/>
     </row>
-    <row r="25" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>30</v>
       </c>
@@ -10398,7 +11439,7 @@
       <c r="FJ25" s="21"/>
       <c r="FK25" s="21"/>
     </row>
-    <row r="26" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>31</v>
       </c>
@@ -10749,7 +11790,7 @@
       <c r="FJ26" s="21"/>
       <c r="FK26" s="21"/>
     </row>
-    <row r="27" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>32</v>
       </c>
@@ -11100,7 +12141,7 @@
       <c r="FJ27" s="21"/>
       <c r="FK27" s="21"/>
     </row>
-    <row r="28" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>33</v>
       </c>
@@ -11451,7 +12492,7 @@
       <c r="FJ28" s="21"/>
       <c r="FK28" s="21"/>
     </row>
-    <row r="29" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>34</v>
       </c>
@@ -11802,7 +12843,7 @@
       <c r="FJ29" s="21"/>
       <c r="FK29" s="21"/>
     </row>
-    <row r="30" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>35</v>
       </c>
@@ -12153,7 +13194,7 @@
       <c r="FJ30" s="21"/>
       <c r="FK30" s="21"/>
     </row>
-    <row r="31" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>36</v>
       </c>
@@ -12504,7 +13545,7 @@
       <c r="FJ31" s="21"/>
       <c r="FK31" s="21"/>
     </row>
-    <row r="32" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>37</v>
       </c>
@@ -12855,7 +13896,7 @@
       <c r="FJ32" s="21"/>
       <c r="FK32" s="21"/>
     </row>
-    <row r="33" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>38</v>
       </c>
@@ -13206,7 +14247,7 @@
       <c r="FJ33" s="21"/>
       <c r="FK33" s="21"/>
     </row>
-    <row r="34" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>39</v>
       </c>
@@ -13557,7 +14598,7 @@
       <c r="FJ34" s="21"/>
       <c r="FK34" s="21"/>
     </row>
-    <row r="35" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>40</v>
       </c>
@@ -13908,7 +14949,7 @@
       <c r="FJ35" s="21"/>
       <c r="FK35" s="21"/>
     </row>
-    <row r="36" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>41</v>
       </c>
@@ -14259,7 +15300,7 @@
       <c r="FJ36" s="21"/>
       <c r="FK36" s="21"/>
     </row>
-    <row r="37" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>42</v>
       </c>
@@ -14610,7 +15651,7 @@
       <c r="FJ37" s="21"/>
       <c r="FK37" s="21"/>
     </row>
-    <row r="38" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>43</v>
       </c>
@@ -14961,7 +16002,7 @@
       <c r="FJ38" s="21"/>
       <c r="FK38" s="21"/>
     </row>
-    <row r="39" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>44</v>
       </c>
@@ -15312,7 +16353,7 @@
       <c r="FJ39" s="21"/>
       <c r="FK39" s="21"/>
     </row>
-    <row r="40" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>45</v>
       </c>
@@ -15663,7 +16704,7 @@
       <c r="FJ40" s="21"/>
       <c r="FK40" s="21"/>
     </row>
-    <row r="41" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>46</v>
       </c>
@@ -16014,7 +17055,7 @@
       <c r="FJ41" s="21"/>
       <c r="FK41" s="21"/>
     </row>
-    <row r="42" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>47</v>
       </c>
@@ -16365,7 +17406,7 @@
       <c r="FJ42" s="21"/>
       <c r="FK42" s="21"/>
     </row>
-    <row r="43" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>48</v>
       </c>
@@ -16716,7 +17757,7 @@
       <c r="FJ43" s="21"/>
       <c r="FK43" s="21"/>
     </row>
-    <row r="44" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>49</v>
       </c>
@@ -17067,7 +18108,7 @@
       <c r="FJ44" s="21"/>
       <c r="FK44" s="21"/>
     </row>
-    <row r="45" spans="1:167" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:167" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>50</v>
       </c>
@@ -17418,7 +18459,7 @@
       <c r="FJ45" s="21"/>
       <c r="FK45" s="21"/>
     </row>
-    <row r="46" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>51</v>
       </c>
@@ -17769,7 +18810,7 @@
       <c r="FJ46" s="21"/>
       <c r="FK46" s="21"/>
     </row>
-    <row r="47" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>52</v>
       </c>
@@ -18120,7 +19161,7 @@
       <c r="FJ47" s="21"/>
       <c r="FK47" s="21"/>
     </row>
-    <row r="48" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>53</v>
       </c>
@@ -18471,7 +19512,7 @@
       <c r="FJ48" s="21"/>
       <c r="FK48" s="21"/>
     </row>
-    <row r="49" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>54</v>
       </c>
@@ -18822,7 +19863,7 @@
       <c r="FJ49" s="21"/>
       <c r="FK49" s="21"/>
     </row>
-    <row r="50" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>55</v>
       </c>
@@ -19173,7 +20214,7 @@
       <c r="FJ50" s="21"/>
       <c r="FK50" s="21"/>
     </row>
-    <row r="51" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>56</v>
       </c>
@@ -19524,7 +20565,7 @@
       <c r="FJ51" s="21"/>
       <c r="FK51" s="21"/>
     </row>
-    <row r="52" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>57</v>
       </c>
@@ -19875,7 +20916,7 @@
       <c r="FJ52" s="21"/>
       <c r="FK52" s="21"/>
     </row>
-    <row r="53" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>58</v>
       </c>
@@ -20226,7 +21267,7 @@
       <c r="FJ53" s="21"/>
       <c r="FK53" s="21"/>
     </row>
-    <row r="54" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>59</v>
       </c>
@@ -20577,7 +21618,7 @@
       <c r="FJ54" s="21"/>
       <c r="FK54" s="21"/>
     </row>
-    <row r="55" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>60</v>
       </c>
@@ -20928,7 +21969,7 @@
       <c r="FJ55" s="21"/>
       <c r="FK55" s="21"/>
     </row>
-    <row r="56" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>61</v>
       </c>
@@ -21279,7 +22320,7 @@
       <c r="FJ56" s="21"/>
       <c r="FK56" s="21"/>
     </row>
-    <row r="57" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>62</v>
       </c>
@@ -21630,7 +22671,7 @@
       <c r="FJ57" s="21"/>
       <c r="FK57" s="21"/>
     </row>
-    <row r="58" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>63</v>
       </c>
@@ -21981,7 +23022,7 @@
       <c r="FJ58" s="21"/>
       <c r="FK58" s="21"/>
     </row>
-    <row r="59" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>64</v>
       </c>
@@ -22332,7 +23373,7 @@
       <c r="FJ59" s="21"/>
       <c r="FK59" s="21"/>
     </row>
-    <row r="60" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>65</v>
       </c>
@@ -22683,7 +23724,7 @@
       <c r="FJ60" s="21"/>
       <c r="FK60" s="21"/>
     </row>
-    <row r="61" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>66</v>
       </c>
@@ -23034,7 +24075,7 @@
       <c r="FJ61" s="21"/>
       <c r="FK61" s="21"/>
     </row>
-    <row r="62" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>67</v>
       </c>
@@ -23385,7 +24426,7 @@
       <c r="FJ62" s="21"/>
       <c r="FK62" s="21"/>
     </row>
-    <row r="63" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>68</v>
       </c>
@@ -23736,7 +24777,7 @@
       <c r="FJ63" s="21"/>
       <c r="FK63" s="21"/>
     </row>
-    <row r="64" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>69</v>
       </c>
@@ -24087,7 +25128,7 @@
       <c r="FJ64" s="21"/>
       <c r="FK64" s="21"/>
     </row>
-    <row r="65" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>70</v>
       </c>
@@ -24438,7 +25479,7 @@
       <c r="FJ65" s="21"/>
       <c r="FK65" s="21"/>
     </row>
-    <row r="66" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>71</v>
       </c>
@@ -24789,7 +25830,7 @@
       <c r="FJ66" s="21"/>
       <c r="FK66" s="21"/>
     </row>
-    <row r="67" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>72</v>
       </c>
@@ -25140,7 +26181,7 @@
       <c r="FJ67" s="21"/>
       <c r="FK67" s="21"/>
     </row>
-    <row r="68" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>73</v>
       </c>
@@ -25491,7 +26532,7 @@
       <c r="FJ68" s="21"/>
       <c r="FK68" s="21"/>
     </row>
-    <row r="69" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>74</v>
       </c>
@@ -25842,7 +26883,7 @@
       <c r="FJ69" s="21"/>
       <c r="FK69" s="21"/>
     </row>
-    <row r="70" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>75</v>
       </c>
@@ -26193,7 +27234,7 @@
       <c r="FJ70" s="21"/>
       <c r="FK70" s="21"/>
     </row>
-    <row r="71" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>76</v>
       </c>
@@ -26544,7 +27585,7 @@
       <c r="FJ71" s="21"/>
       <c r="FK71" s="21"/>
     </row>
-    <row r="72" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>77</v>
       </c>
@@ -26895,7 +27936,7 @@
       <c r="FJ72" s="21"/>
       <c r="FK72" s="21"/>
     </row>
-    <row r="73" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>78</v>
       </c>
@@ -27246,7 +28287,7 @@
       <c r="FJ73" s="21"/>
       <c r="FK73" s="21"/>
     </row>
-    <row r="74" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>79</v>
       </c>
@@ -27597,7 +28638,7 @@
       <c r="FJ74" s="21"/>
       <c r="FK74" s="21"/>
     </row>
-    <row r="75" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>80</v>
       </c>
@@ -27948,7 +28989,7 @@
       <c r="FJ75" s="21"/>
       <c r="FK75" s="21"/>
     </row>
-    <row r="76" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>81</v>
       </c>
@@ -28299,7 +29340,7 @@
       <c r="FJ76" s="21"/>
       <c r="FK76" s="21"/>
     </row>
-    <row r="77" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>82</v>
       </c>
@@ -28650,7 +29691,7 @@
       <c r="FJ77" s="21"/>
       <c r="FK77" s="21"/>
     </row>
-    <row r="78" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>83</v>
       </c>
@@ -29001,7 +30042,7 @@
       <c r="FJ78" s="21"/>
       <c r="FK78" s="21"/>
     </row>
-    <row r="79" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>84</v>
       </c>
@@ -29352,7 +30393,7 @@
       <c r="FJ79" s="21"/>
       <c r="FK79" s="21"/>
     </row>
-    <row r="80" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>85</v>
       </c>
@@ -29703,7 +30744,7 @@
       <c r="FJ80" s="21"/>
       <c r="FK80" s="21"/>
     </row>
-    <row r="81" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>86</v>
       </c>
@@ -30054,7 +31095,7 @@
       <c r="FJ81" s="21"/>
       <c r="FK81" s="21"/>
     </row>
-    <row r="82" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>87</v>
       </c>
@@ -30405,7 +31446,7 @@
       <c r="FJ82" s="21"/>
       <c r="FK82" s="21"/>
     </row>
-    <row r="83" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>88</v>
       </c>
@@ -30756,7 +31797,7 @@
       <c r="FJ83" s="21"/>
       <c r="FK83" s="21"/>
     </row>
-    <row r="84" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>89</v>
       </c>
@@ -31107,7 +32148,7 @@
       <c r="FJ84" s="21"/>
       <c r="FK84" s="21"/>
     </row>
-    <row r="85" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>90</v>
       </c>
@@ -31458,7 +32499,7 @@
       <c r="FJ85" s="21"/>
       <c r="FK85" s="21"/>
     </row>
-    <row r="86" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>91</v>
       </c>
@@ -31809,7 +32850,7 @@
       <c r="FJ86" s="21"/>
       <c r="FK86" s="21"/>
     </row>
-    <row r="87" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>92</v>
       </c>
@@ -32160,7 +33201,7 @@
       <c r="FJ87" s="21"/>
       <c r="FK87" s="21"/>
     </row>
-    <row r="88" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>93</v>
       </c>
@@ -32511,7 +33552,7 @@
       <c r="FJ88" s="21"/>
       <c r="FK88" s="21"/>
     </row>
-    <row r="89" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>94</v>
       </c>
@@ -32862,7 +33903,7 @@
       <c r="FJ89" s="21"/>
       <c r="FK89" s="21"/>
     </row>
-    <row r="90" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>95</v>
       </c>
@@ -33213,7 +34254,7 @@
       <c r="FJ90" s="21"/>
       <c r="FK90" s="21"/>
     </row>
-    <row r="91" spans="1:167" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:167" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>96</v>
       </c>
@@ -33564,35 +34605,35 @@
       <c r="FJ91" s="21"/>
       <c r="FK91" s="21"/>
     </row>
-    <row r="92" spans="1:167" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:167" x14ac:dyDescent="0.2">
       <c r="CL92" s="21"/>
       <c r="CM92" s="21"/>
       <c r="CN92" s="21"/>
       <c r="CO92" s="21"/>
       <c r="CP92" s="21"/>
     </row>
-    <row r="93" spans="1:167" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:167" x14ac:dyDescent="0.2">
       <c r="CL93" s="21"/>
       <c r="CM93" s="21"/>
       <c r="CN93" s="21"/>
       <c r="CO93" s="21"/>
       <c r="CP93" s="21"/>
     </row>
-    <row r="94" spans="1:167" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:167" x14ac:dyDescent="0.2">
       <c r="CL94" s="21"/>
       <c r="CM94" s="21"/>
       <c r="CN94" s="21"/>
       <c r="CO94" s="21"/>
       <c r="CP94" s="21"/>
     </row>
-    <row r="95" spans="1:167" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:167" x14ac:dyDescent="0.2">
       <c r="CL95" s="21"/>
       <c r="CM95" s="21"/>
       <c r="CN95" s="21"/>
       <c r="CO95" s="21"/>
       <c r="CP95" s="21"/>
     </row>
-    <row r="96" spans="1:167" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:167" x14ac:dyDescent="0.2">
       <c r="CK96" s="21"/>
       <c r="CL96" s="21"/>
       <c r="CM96" s="21"/>
@@ -33600,7 +34641,7 @@
       <c r="CO96" s="21"/>
       <c r="CP96" s="21"/>
     </row>
-    <row r="97" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="97" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK97" s="21"/>
       <c r="CL97" s="21"/>
       <c r="CM97" s="21"/>
@@ -33608,7 +34649,7 @@
       <c r="CO97" s="21"/>
       <c r="CP97" s="21"/>
     </row>
-    <row r="98" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="98" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK98" s="21"/>
       <c r="CL98" s="21"/>
       <c r="CM98" s="21"/>
@@ -33616,7 +34657,7 @@
       <c r="CO98" s="21"/>
       <c r="CP98" s="21"/>
     </row>
-    <row r="99" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="99" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK99" s="21"/>
       <c r="CL99" s="21"/>
       <c r="CM99" s="21"/>
@@ -33624,28 +34665,28 @@
       <c r="CO99" s="21"/>
       <c r="CP99" s="21"/>
     </row>
-    <row r="100" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="100" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK100" s="21"/>
       <c r="CL100" s="21"/>
       <c r="CM100" s="21"/>
       <c r="CN100" s="21"/>
       <c r="CO100" s="21"/>
     </row>
-    <row r="101" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="101" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK101" s="21"/>
       <c r="CL101" s="21"/>
       <c r="CM101" s="21"/>
       <c r="CN101" s="21"/>
       <c r="CO101" s="21"/>
     </row>
-    <row r="102" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="102" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK102" s="21"/>
       <c r="CL102" s="21"/>
       <c r="CM102" s="21"/>
       <c r="CN102" s="21"/>
       <c r="CO102" s="21"/>
     </row>
-    <row r="103" spans="89:94" x14ac:dyDescent="0.25">
+    <row r="103" spans="89:94" x14ac:dyDescent="0.2">
       <c r="CK103" s="21"/>
       <c r="CL103" s="21"/>
       <c r="CM103" s="21"/>
@@ -33657,21 +34698,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection sqref="A1:A92"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -33694,7 +34735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -33718,7 +34759,7 @@
         <v>10706.740000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -33742,7 +34783,7 @@
         <v>5986.09</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -33766,7 +34807,7 @@
         <v>2841.14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -33790,7 +34831,7 @@
         <v>966.62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -33814,7 +34855,7 @@
         <v>16183.099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -33838,7 +34879,7 @@
         <v>1752.13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -33862,7 +34903,7 @@
         <v>74243.259999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -33886,7 +34927,7 @@
         <v>48367.09</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -33910,7 +34951,7 @@
         <v>2611.52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -33934,7 +34975,7 @@
         <v>4373.2699999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -33958,7 +34999,7 @@
         <v>4018.67</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -33982,7 +35023,7 @@
         <v>27303.46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -34006,7 +35047,7 @@
         <v>7856.0199999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -34030,7 +35071,7 @@
         <v>764.81000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -34054,7 +35095,7 @@
         <v>75923.81</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -34078,7 +35119,7 @@
         <v>729.26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34102,7 +35143,7 @@
         <v>18566.580000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
@@ -34126,7 +35167,7 @@
         <v>5401.67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -34150,7 +35191,7 @@
         <v>2209.0500000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -34174,7 +35215,7 @@
         <v>10183.25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -34198,7 +35239,7 @@
         <v>279.25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -34222,7 +35263,7 @@
         <v>505.98</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -34246,7 +35287,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -34270,7 +35311,7 @@
         <v>5327.77</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -34294,7 +35335,7 @@
         <v>5395.25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -34318,7 +35359,7 @@
         <v>4402.1099999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
@@ -34342,7 +35383,7 @@
         <v>1394.51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
@@ -34366,7 +35407,7 @@
         <v>1397.6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -34390,7 +35431,7 @@
         <v>6923.0599999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>36</v>
       </c>
@@ -34414,7 +35455,7 @@
         <v>17840.16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>37</v>
       </c>
@@ -34438,7 +35479,7 @@
         <v>3744.4800000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>38</v>
       </c>
@@ -34462,7 +35503,7 @@
         <v>1485.91</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
@@ -34486,7 +35527,7 @@
         <v>3974.77</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>40</v>
       </c>
@@ -34510,7 +35551,7 @@
         <v>1782.33</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
@@ -34534,7 +35575,7 @@
         <v>722.43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -34558,7 +35599,7 @@
         <v>46210.92</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
@@ -34582,7 +35623,7 @@
         <v>12290.8</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
@@ -34606,7 +35647,7 @@
         <v>11138.25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
@@ -34630,7 +35671,7 @@
         <v>44886.789999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
@@ -34654,7 +35695,7 @@
         <v>5318.21</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
@@ -34678,7 +35719,7 @@
         <v>2852.75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -34702,7 +35743,7 @@
         <v>6045.01</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -34726,7 +35767,7 @@
         <v>6978.2600000000011</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -34750,7 +35791,7 @@
         <v>2031.79</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
@@ -34774,7 +35815,7 @@
         <v>4487.42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -34798,7 +35839,7 @@
         <v>3626.19</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>53</v>
       </c>
@@ -34822,7 +35863,7 @@
         <v>897.5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>54</v>
       </c>
@@ -34846,7 +35887,7 @@
         <v>757.71</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
@@ -34870,7 +35911,7 @@
         <v>7526.5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
@@ -34894,7 +35935,7 @@
         <v>5433.8600000000006</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
@@ -34918,7 +35959,7 @@
         <v>4396.97</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>58</v>
       </c>
@@ -34942,7 +35983,7 @@
         <v>989.07</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>59</v>
       </c>
@@ -34966,7 +36007,7 @@
         <v>9360.07</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>60</v>
       </c>
@@ -34990,7 +36031,7 @@
         <v>6602.52</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>61</v>
       </c>
@@ -35014,7 +36055,7 @@
         <v>2520.9900000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>62</v>
       </c>
@@ -35038,7 +36079,7 @@
         <v>1649.0200000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>63</v>
       </c>
@@ -35062,7 +36103,7 @@
         <v>902.07999999999993</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>64</v>
       </c>
@@ -35092,7 +36133,7 @@
         <v>1452.26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>65</v>
       </c>
@@ -35116,7 +36157,7 @@
         <v>650.95000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>66</v>
       </c>
@@ -35140,7 +36181,7 @@
         <v>683.56</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
@@ -35164,7 +36205,7 @@
         <v>1530.1299999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>68</v>
       </c>
@@ -35188,7 +36229,7 @@
         <v>10274.280000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -35212,7 +36253,7 @@
         <v>10073.799999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>70</v>
       </c>
@@ -35236,7 +36277,7 @@
         <v>2857.96</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
@@ -35260,7 +36301,7 @@
         <v>62367.81</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>72</v>
       </c>
@@ -35284,7 +36325,7 @@
         <v>690.33999999999992</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>73</v>
       </c>
@@ -35308,7 +36349,7 @@
         <v>6507.7400000000016</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>74</v>
       </c>
@@ -35332,7 +36373,7 @@
         <v>18450.23</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>75</v>
       </c>
@@ -35356,7 +36397,7 @@
         <v>934.53000000000009</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>76</v>
       </c>
@@ -35380,7 +36421,7 @@
         <v>89920.67</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>77</v>
       </c>
@@ -35404,7 +36445,7 @@
         <v>4511.78</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>78</v>
       </c>
@@ -35428,7 +36469,7 @@
         <v>103481.49</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>79</v>
       </c>
@@ -35452,7 +36493,7 @@
         <v>349.04</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>80</v>
       </c>
@@ -35476,7 +36517,7 @@
         <v>2625.98</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>81</v>
       </c>
@@ -35500,7 +36541,7 @@
         <v>1113.92</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>82</v>
       </c>
@@ -35524,7 +36565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>83</v>
       </c>
@@ -35548,7 +36589,7 @@
         <v>7270.65</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>84</v>
       </c>
@@ -35572,7 +36613,7 @@
         <v>8519.33</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>85</v>
       </c>
@@ -35596,7 +36637,7 @@
         <v>3956.09</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>86</v>
       </c>
@@ -35620,7 +36661,7 @@
         <v>34145.06</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>87</v>
       </c>
@@ -35644,7 +36685,7 @@
         <v>1021.22</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>88</v>
       </c>
@@ -35668,7 +36709,7 @@
         <v>3247.53</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>89</v>
       </c>
@@ -35692,7 +36733,7 @@
         <v>176432.78999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>90</v>
       </c>
@@ -35716,7 +36757,7 @@
         <v>4746.8899999999994</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>91</v>
       </c>
@@ -35740,7 +36781,7 @@
         <v>6708.57</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>92</v>
       </c>
@@ -35764,7 +36805,7 @@
         <v>7705.2799999999988</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>93</v>
       </c>
@@ -35788,7 +36829,7 @@
         <v>3471.9399999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>94</v>
       </c>
@@ -35812,7 +36853,7 @@
         <v>11453.73</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>95</v>
       </c>
@@ -35836,7 +36877,7 @@
         <v>5917.6900000000005</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>96</v>
       </c>
@@ -35860,7 +36901,7 @@
         <v>11174.61</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>97</v>
       </c>
@@ -35893,7 +36934,7 @@
         <v>1168293.67</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F93">
         <v>230971.35</v>
       </c>

</xml_diff>